<commit_message>
add - management command - auth_user_groups
</commit_message>
<xml_diff>
--- a/core/seed_auth_group.xlsx
+++ b/core/seed_auth_group.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.cheng\Documents\Visual Studio Code\Django\p_sys01_repo01\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BA2322-9290-45B1-9475-5CA0FE0EFFA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8412CB-EB81-43D0-AECD-791D17E32ECE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -893,7 +893,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update - generate dummy transactions
</commit_message>
<xml_diff>
--- a/core/seed_auth_group.xlsx
+++ b/core/seed_auth_group.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.cheng\Documents\Visual Studio Code\Django\p_sys01_repo01\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8412CB-EB81-43D0-AECD-791D17E32ECE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A614601B-253E-4F14-8C7A-88154BAAC6B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -893,7 +893,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>